<commit_message>
Golaiths project is published!
</commit_message>
<xml_diff>
--- a/data/role-mnc.xlsx
+++ b/data/role-mnc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/global-goliaths/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3ED147-EBD6-8743-A35E-DA7814BF64C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2097325-FBB4-794B-BC05-1ACA3A2E3C45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" xr2:uid="{040CBE59-C8FA-694F-8BEB-1A8834E7EBE6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Figure 1: The Role of Multinational Firms in the U.S. Economy, 2017</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>mnc_type</t>
+  </si>
+  <si>
+    <t>Employee Compensation</t>
+  </si>
+  <si>
+    <t>Manufacturing Employee Compensation</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2282,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2294,13 +2300,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>16</v>

</xml_diff>